<commit_message>
tickets, fix recaptcha style,
</commit_message>
<xml_diff>
--- a/MIA/ClientApp/locales_data.xlsx
+++ b/MIA/ClientApp/locales_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
   <si>
     <t>msgid</t>
   </si>
@@ -70,9 +70,6 @@
     <t>award_category</t>
   </si>
   <si>
-    <t>award category</t>
-  </si>
-  <si>
     <t>awards</t>
   </si>
   <si>
@@ -166,9 +163,6 @@
     <t>country</t>
   </si>
   <si>
-    <t>Country</t>
-  </si>
-  <si>
     <t>create_account</t>
   </si>
   <si>
@@ -226,9 +220,6 @@
     <t>genre</t>
   </si>
   <si>
-    <t>Genre</t>
-  </si>
-  <si>
     <t>get_in_touch</t>
   </si>
   <si>
@@ -337,6 +328,66 @@
     <t>Old password</t>
   </si>
   <si>
+    <t>our_awards</t>
+  </si>
+  <si>
+    <t>Our Awards</t>
+  </si>
+  <si>
+    <t>our_awards_text</t>
+  </si>
+  <si>
+    <t>The Arab Media Makers Award (MIA 2020), which is judged among contestants electronically, aims to measure the quality of the level of influence of the content of TV works on the lifestyle, audience thinking and impact by sorting the participating works according to specific conditions and criteria by the jury, and we have dedicated to each Category of the competition is three gold, silver and bronze prizes distributed to the winners with appreciation certificates</t>
+  </si>
+  <si>
+    <t>our_events</t>
+  </si>
+  <si>
+    <t>Our Events</t>
+  </si>
+  <si>
+    <t>our_events_text</t>
+  </si>
+  <si>
+    <t>&lt;0&gt;&lt;1&gt;• Workshops to develop technical and technical professional capabilities&lt;/1&gt;&lt;2&gt;• Specialized seminars, to be hosted by experts and professionals from the media makers and Arab art stars&lt;/2&gt;&lt;3&gt;• View distinctive success stories&lt;/3&gt;&lt;4&gt;• Market for the most recent engineering and technical systems in the field of media and television production&lt;/4&gt;&lt;5&gt;• TV interviews discussing important issues (live broadcast)&lt;/5&gt;&lt;/0&gt;</t>
+  </si>
+  <si>
+    <t>our_goal</t>
+  </si>
+  <si>
+    <t>Our Goal</t>
+  </si>
+  <si>
+    <t>our_goal_text</t>
+  </si>
+  <si>
+    <t>&lt;0&gt;&lt;1&gt;• Upgrading the taste of the Arab person in its various segments, and presenting new future visions that contribute to advancing the future of Arab TV production.&lt;/1&gt;&lt;2&gt;• Activating and stimulating the TV content industry and raising the level of Arab production and promoting it to international ranks&lt;/2&gt;&lt;3&gt;• Finding an opportunity for integration, interaction and the convergence of multiple cultures in order to integrate the Arab identity, so that we can together create a brilliant future With One Power and Promising Generations&lt;/3&gt;&lt;4&gt;• Increasing the communication between the young talents in the Arab world and the elite producers and technicians working in the field and providing the greatest degree of integration between the productive sectors and between the media organizations and TV channels&lt;/4&gt;&lt;5&gt;• Discover new talents and show distinguished ones to the limelight&lt;/5&gt;&lt;6&gt;• Appreciating and honoring the creators and accomplished people throughout the Arab world by evaluating their work, knowing the opinions of the specialists about it and celebrating its best.&lt;/6&gt;&lt;/0&gt;</t>
+  </si>
+  <si>
+    <t>our_message</t>
+  </si>
+  <si>
+    <t>Our Message</t>
+  </si>
+  <si>
+    <t>our_message_text</t>
+  </si>
+  <si>
+    <t>Recent studies have proven the importance of television content in our daily lives and its influence on changing values ​​and cultural awareness in any society. It is for this importance that our message was launched from the slogan of our slogan (Arab media is a new reality) to raise the level of quality content in Arab television production and make this award an Arab platform that honors and meets all the distinguished and creative in this field, during which new ideas converge and lead to a knowledge and technical product that Arab societies benefit from and confront with it Its various future challenges</t>
+  </si>
+  <si>
+    <t>our_value</t>
+  </si>
+  <si>
+    <t>our value</t>
+  </si>
+  <si>
+    <t>our_value_text</t>
+  </si>
+  <si>
+    <t>&lt;0&gt;&lt;1&gt;&lt;2&gt;• Neutrality :&lt;/2&gt;&lt;3&gt;We stand without siding and one distance from all the people of the Arab world&lt;/3&gt;&lt;/1&gt;&lt;4&gt;&lt;5&gt;• Objectivity :&lt;/5&gt;&lt;6&gt;Away from the whims, one mechanism in dealing with each performance. &lt;7/&gt; Your creativity determines your position&lt;/6&gt;&lt;/4&gt;&lt;8&gt;&lt;9&gt;• Credibility :&lt;/9&gt;&lt;10&gt;One of the basic principles of our work .. Our integrity is our method in our evaluation&lt;/10&gt;&lt;/8&gt;&lt;11&gt;&lt;12&gt;• Enhancement :&lt;/12&gt;&lt;13&gt;Providing numerous quality awards and discretionary seals according to performance criteria&lt;/13&gt;&lt;/11&gt;&lt;/0&gt;</t>
+  </si>
+  <si>
     <t>phone</t>
   </si>
   <si>
@@ -470,6 +521,18 @@
   </si>
   <si>
     <t>starts from</t>
+  </si>
+  <si>
+    <t>story</t>
+  </si>
+  <si>
+    <t>Story</t>
+  </si>
+  <si>
+    <t>story_text</t>
+  </si>
+  <si>
+    <t>The Arab media passes during the past decades a lot of challenges and the lack of representation of the Arab reality with the correct representation, despite the presence of a large investment in the field of media in all its forms, but it lacks concerted efforts between investors and production companies. Art making and Arab business production by being the link between the investor and the producer in order to transfer the Arab "television" reality to the right path by creating an award for visual media, believing that the competition will create rich and distinctive content that will affect its audience. Dowries and recipients in the Arab world</t>
   </si>
   <si>
     <t>submit</t>
@@ -601,7 +664,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomRight" state="frozen"/>
@@ -757,7 +820,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>7</v>
@@ -771,13 +834,13 @@
     </row>
     <row r="9" spans="1:6" customHeight="1">
       <c r="A9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>21</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>7</v>
@@ -791,13 +854,13 @@
     </row>
     <row r="10" spans="1:6" customHeight="1">
       <c r="A10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>23</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>7</v>
@@ -811,7 +874,7 @@
     </row>
     <row r="11" spans="1:6" customHeight="1">
       <c r="A11" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>7</v>
@@ -831,13 +894,13 @@
     </row>
     <row r="12" spans="1:6" customHeight="1">
       <c r="A12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>7</v>
@@ -851,13 +914,13 @@
     </row>
     <row r="13" spans="1:6" customHeight="1">
       <c r="A13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>28</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>7</v>
@@ -871,13 +934,13 @@
     </row>
     <row r="14" spans="1:6" customHeight="1">
       <c r="A14" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>30</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>7</v>
@@ -891,13 +954,13 @@
     </row>
     <row r="15" spans="1:6" customHeight="1">
       <c r="A15" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>32</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>7</v>
@@ -911,13 +974,13 @@
     </row>
     <row r="16" spans="1:6" customHeight="1">
       <c r="A16" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>7</v>
@@ -931,13 +994,13 @@
     </row>
     <row r="17" spans="1:6" customHeight="1">
       <c r="A17" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>36</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>7</v>
@@ -951,13 +1014,13 @@
     </row>
     <row r="18" spans="1:6" customHeight="1">
       <c r="A18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>7</v>
@@ -971,13 +1034,13 @@
     </row>
     <row r="19" spans="1:6" customHeight="1">
       <c r="A19" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>40</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>7</v>
@@ -991,13 +1054,13 @@
     </row>
     <row r="20" spans="1:6" customHeight="1">
       <c r="A20" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>42</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>7</v>
@@ -1011,13 +1074,13 @@
     </row>
     <row r="21" spans="1:6" customHeight="1">
       <c r="A21" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>7</v>
@@ -1031,13 +1094,13 @@
     </row>
     <row r="22" spans="1:6" customHeight="1">
       <c r="A22" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>7</v>
@@ -1051,13 +1114,13 @@
     </row>
     <row r="23" spans="1:6" customHeight="1">
       <c r="A23" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>47</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>7</v>
@@ -1071,13 +1134,13 @@
     </row>
     <row r="24" spans="1:6" customHeight="1">
       <c r="A24" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>49</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>7</v>
@@ -1091,13 +1154,13 @@
     </row>
     <row r="25" spans="1:6" customHeight="1">
       <c r="A25" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>7</v>
@@ -1111,13 +1174,13 @@
     </row>
     <row r="26" spans="1:6" customHeight="1">
       <c r="A26" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>7</v>
@@ -1131,13 +1194,13 @@
     </row>
     <row r="27" spans="1:6" customHeight="1">
       <c r="A27" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>7</v>
@@ -1151,13 +1214,13 @@
     </row>
     <row r="28" spans="1:6" customHeight="1">
       <c r="A28" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>7</v>
@@ -1171,13 +1234,13 @@
     </row>
     <row r="29" spans="1:6" customHeight="1">
       <c r="A29" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>7</v>
@@ -1191,13 +1254,13 @@
     </row>
     <row r="30" spans="1:6" customHeight="1">
       <c r="A30" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>7</v>
@@ -1211,13 +1274,13 @@
     </row>
     <row r="31" spans="1:6" customHeight="1">
       <c r="A31" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>7</v>
@@ -1231,13 +1294,13 @@
     </row>
     <row r="32" spans="1:6" customHeight="1">
       <c r="A32" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>7</v>
@@ -1251,13 +1314,13 @@
     </row>
     <row r="33" spans="1:6" customHeight="1">
       <c r="A33" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>7</v>
@@ -1271,13 +1334,13 @@
     </row>
     <row r="34" spans="1:6" customHeight="1">
       <c r="A34" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>7</v>
@@ -1291,13 +1354,13 @@
     </row>
     <row r="35" spans="1:6" customHeight="1">
       <c r="A35" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>7</v>
@@ -1311,13 +1374,13 @@
     </row>
     <row r="36" spans="1:6" customHeight="1">
       <c r="A36" s="0" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>7</v>
@@ -1331,13 +1394,13 @@
     </row>
     <row r="37" spans="1:6" customHeight="1">
       <c r="A37" s="0" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>7</v>
@@ -1351,13 +1414,13 @@
     </row>
     <row r="38" spans="1:6" customHeight="1">
       <c r="A38" s="0" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>7</v>
@@ -1371,13 +1434,13 @@
     </row>
     <row r="39" spans="1:6" customHeight="1">
       <c r="A39" s="0" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>7</v>
@@ -1391,7 +1454,7 @@
     </row>
     <row r="40" spans="1:6" customHeight="1">
       <c r="A40" s="0" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>7</v>
@@ -1411,13 +1474,13 @@
     </row>
     <row r="41" spans="1:6" customHeight="1">
       <c r="A41" s="0" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>7</v>
@@ -1431,13 +1494,13 @@
     </row>
     <row r="42" spans="1:6" customHeight="1">
       <c r="A42" s="0" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>7</v>
@@ -1451,13 +1514,13 @@
     </row>
     <row r="43" spans="1:6" customHeight="1">
       <c r="A43" s="0" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>7</v>
@@ -1471,13 +1534,13 @@
     </row>
     <row r="44" spans="1:6" customHeight="1">
       <c r="A44" s="0" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>7</v>
@@ -1491,13 +1554,13 @@
     </row>
     <row r="45" spans="1:6" customHeight="1">
       <c r="A45" s="0" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>7</v>
@@ -1511,13 +1574,13 @@
     </row>
     <row r="46" spans="1:6" customHeight="1">
       <c r="A46" s="0" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>7</v>
@@ -1531,13 +1594,13 @@
     </row>
     <row r="47" spans="1:6" customHeight="1">
       <c r="A47" s="0" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>7</v>
@@ -1551,13 +1614,13 @@
     </row>
     <row r="48" spans="1:6" customHeight="1">
       <c r="A48" s="0" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>7</v>
@@ -1571,13 +1634,13 @@
     </row>
     <row r="49" spans="1:6" customHeight="1">
       <c r="A49" s="0" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>7</v>
@@ -1591,13 +1654,13 @@
     </row>
     <row r="50" spans="1:6" customHeight="1">
       <c r="A50" s="0" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>7</v>
@@ -1611,13 +1674,13 @@
     </row>
     <row r="51" spans="1:6" customHeight="1">
       <c r="A51" s="0" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>7</v>
@@ -1631,13 +1694,13 @@
     </row>
     <row r="52" spans="1:6" customHeight="1">
       <c r="A52" s="0" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>7</v>
@@ -1651,7 +1714,7 @@
     </row>
     <row r="53" spans="1:6" customHeight="1">
       <c r="A53" s="0" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>7</v>
@@ -1671,13 +1734,13 @@
     </row>
     <row r="54" spans="1:6" customHeight="1">
       <c r="A54" s="0" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>7</v>
@@ -1691,13 +1754,13 @@
     </row>
     <row r="55" spans="1:6" customHeight="1">
       <c r="A55" s="0" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>7</v>
@@ -1711,13 +1774,13 @@
     </row>
     <row r="56" spans="1:6" customHeight="1">
       <c r="A56" s="0" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>7</v>
@@ -1731,13 +1794,13 @@
     </row>
     <row r="57" spans="1:6" customHeight="1">
       <c r="A57" s="0" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>7</v>
@@ -1751,13 +1814,13 @@
     </row>
     <row r="58" spans="1:6" customHeight="1">
       <c r="A58" s="0" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>7</v>
@@ -1771,13 +1834,13 @@
     </row>
     <row r="59" spans="1:6" customHeight="1">
       <c r="A59" s="0" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>7</v>
@@ -1791,13 +1854,13 @@
     </row>
     <row r="60" spans="1:6" customHeight="1">
       <c r="A60" s="0" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>7</v>
@@ -1811,13 +1874,13 @@
     </row>
     <row r="61" spans="1:6" customHeight="1">
       <c r="A61" s="0" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>7</v>
@@ -1831,13 +1894,13 @@
     </row>
     <row r="62" spans="1:6" customHeight="1">
       <c r="A62" s="0" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>7</v>
+        <v>120</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>7</v>
@@ -1851,13 +1914,13 @@
     </row>
     <row r="63" spans="1:6" customHeight="1">
       <c r="A63" s="0" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>7</v>
@@ -1871,13 +1934,13 @@
     </row>
     <row r="64" spans="1:6" customHeight="1">
       <c r="A64" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>7</v>
@@ -1891,7 +1954,7 @@
     </row>
     <row r="65" spans="1:6" customHeight="1">
       <c r="A65" s="0" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>7</v>
@@ -1911,13 +1974,13 @@
     </row>
     <row r="66" spans="1:6" customHeight="1">
       <c r="A66" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="B66" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>129</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>7</v>
@@ -1931,13 +1994,13 @@
     </row>
     <row r="67" spans="1:6" customHeight="1">
       <c r="A67" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="0" t="s">
         <v>130</v>
-      </c>
-      <c r="B67" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>131</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>7</v>
@@ -1951,13 +2014,13 @@
     </row>
     <row r="68" spans="1:6" customHeight="1">
       <c r="A68" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="0" t="s">
         <v>132</v>
-      </c>
-      <c r="B68" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>133</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>7</v>
@@ -1971,13 +2034,13 @@
     </row>
     <row r="69" spans="1:6" customHeight="1">
       <c r="A69" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="0" t="s">
         <v>134</v>
-      </c>
-      <c r="B69" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>135</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>7</v>
@@ -1991,13 +2054,13 @@
     </row>
     <row r="70" spans="1:6" customHeight="1">
       <c r="A70" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="0" t="s">
         <v>136</v>
-      </c>
-      <c r="B70" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>137</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>7</v>
@@ -2011,13 +2074,13 @@
     </row>
     <row r="71" spans="1:6" customHeight="1">
       <c r="A71" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="0" t="s">
         <v>138</v>
-      </c>
-      <c r="B71" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>139</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>7</v>
@@ -2031,13 +2094,13 @@
     </row>
     <row r="72" spans="1:6" customHeight="1">
       <c r="A72" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B72" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>141</v>
+        <v>7</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>7</v>
@@ -2051,13 +2114,13 @@
     </row>
     <row r="73" spans="1:6" customHeight="1">
       <c r="A73" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>7</v>
@@ -2071,13 +2134,13 @@
     </row>
     <row r="74" spans="1:6" customHeight="1">
       <c r="A74" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B74" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D74" s="0" t="s">
         <v>7</v>
@@ -2091,13 +2154,13 @@
     </row>
     <row r="75" spans="1:6" customHeight="1">
       <c r="A75" s="0" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D75" s="0" t="s">
         <v>7</v>
@@ -2111,13 +2174,13 @@
     </row>
     <row r="76" spans="1:6" customHeight="1">
       <c r="A76" s="0" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D76" s="0" t="s">
         <v>7</v>
@@ -2131,13 +2194,13 @@
     </row>
     <row r="77" spans="1:6" customHeight="1">
       <c r="A77" s="0" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B77" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>7</v>
+        <v>148</v>
       </c>
       <c r="D77" s="0" t="s">
         <v>7</v>
@@ -2151,13 +2214,13 @@
     </row>
     <row r="78" spans="1:6" customHeight="1">
       <c r="A78" s="0" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B78" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D78" s="0" t="s">
         <v>7</v>
@@ -2171,13 +2234,13 @@
     </row>
     <row r="79" spans="1:6" customHeight="1">
       <c r="A79" s="0" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B79" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D79" s="0" t="s">
         <v>7</v>
@@ -2191,13 +2254,13 @@
     </row>
     <row r="80" spans="1:6" customHeight="1">
       <c r="A80" s="0" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B80" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>7</v>
+        <v>154</v>
       </c>
       <c r="D80" s="0" t="s">
         <v>7</v>
@@ -2211,13 +2274,13 @@
     </row>
     <row r="81" spans="1:6" customHeight="1">
       <c r="A81" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" s="0" t="s">
         <v>156</v>
-      </c>
-      <c r="B81" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C81" s="0" t="s">
-        <v>157</v>
       </c>
       <c r="D81" s="0" t="s">
         <v>7</v>
@@ -2231,13 +2294,13 @@
     </row>
     <row r="82" spans="1:6" customHeight="1">
       <c r="A82" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" s="0" t="s">
         <v>158</v>
-      </c>
-      <c r="B82" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>159</v>
       </c>
       <c r="D82" s="0" t="s">
         <v>7</v>
@@ -2251,13 +2314,13 @@
     </row>
     <row r="83" spans="1:6" customHeight="1">
       <c r="A83" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C83" s="0" t="s">
         <v>160</v>
-      </c>
-      <c r="B83" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="D83" s="0" t="s">
         <v>7</v>
@@ -2337,7 +2400,7 @@
         <v>7</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>168</v>
+        <v>7</v>
       </c>
       <c r="D87" s="0" t="s">
         <v>7</v>
@@ -2351,13 +2414,13 @@
     </row>
     <row r="88" spans="1:6" customHeight="1">
       <c r="A88" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C88" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="B88" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>170</v>
       </c>
       <c r="D88" s="0" t="s">
         <v>7</v>
@@ -2371,13 +2434,13 @@
     </row>
     <row r="89" spans="1:6" customHeight="1">
       <c r="A89" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C89" s="0" t="s">
         <v>171</v>
-      </c>
-      <c r="B89" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C89" s="0" t="s">
-        <v>172</v>
       </c>
       <c r="D89" s="0" t="s">
         <v>7</v>
@@ -2391,13 +2454,13 @@
     </row>
     <row r="90" spans="1:6" customHeight="1">
       <c r="A90" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90" s="0" t="s">
         <v>173</v>
-      </c>
-      <c r="B90" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C90" s="0" t="s">
-        <v>174</v>
       </c>
       <c r="D90" s="0" t="s">
         <v>7</v>
@@ -2411,13 +2474,13 @@
     </row>
     <row r="91" spans="1:6" customHeight="1">
       <c r="A91" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" s="0" t="s">
         <v>175</v>
-      </c>
-      <c r="B91" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C91" s="0" t="s">
-        <v>176</v>
       </c>
       <c r="D91" s="0" t="s">
         <v>7</v>
@@ -2431,21 +2494,261 @@
     </row>
     <row r="92" spans="1:6" customHeight="1">
       <c r="A92" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E92" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F92" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" customHeight="1">
+      <c r="A93" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="B92" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C92" s="0" t="s">
+      <c r="B93" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="D92" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E92" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F92" s="0" t="s">
+      <c r="D93" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E93" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F93" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" customHeight="1">
+      <c r="A94" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="D94" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E94" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F94" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" customHeight="1">
+      <c r="A95" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D95" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E95" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F95" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" customHeight="1">
+      <c r="A96" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="D96" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E96" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F96" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" customHeight="1">
+      <c r="A97" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="D97" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E97" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F97" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" customHeight="1">
+      <c r="A98" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="D98" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E98" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F98" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" customHeight="1">
+      <c r="A99" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E99" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F99" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" customHeight="1">
+      <c r="A100" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D100" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E100" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F100" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" customHeight="1">
+      <c r="A101" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="D101" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E101" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F101" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" customHeight="1">
+      <c r="A102" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="D102" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E102" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F102" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" customHeight="1">
+      <c r="A103" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="D103" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E103" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F103" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" customHeight="1">
+      <c r="A104" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="D104" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E104" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F104" s="0" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>